<commit_message>
working on illumination correction
</commit_message>
<xml_diff>
--- a/Database of all images.xlsx
+++ b/Database of all images.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2178" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2179" uniqueCount="257">
   <si>
     <t>Patient</t>
   </si>
@@ -791,6 +791,9 @@
   </si>
   <si>
     <t>tom gardner results</t>
+  </si>
+  <si>
+    <t>hgdgh</t>
   </si>
 </sst>
 </file>
@@ -1896,11 +1899,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="269851824"/>
-        <c:axId val="272109600"/>
+        <c:axId val="225441728"/>
+        <c:axId val="225442120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="269851824"/>
+        <c:axId val="225441728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1909,7 +1912,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="272109600"/>
+        <c:crossAx val="225442120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1917,7 +1920,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="272109600"/>
+        <c:axId val="225442120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1928,7 +1931,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="269851824"/>
+        <c:crossAx val="225441728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2273,7 +2276,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="T137" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W156" sqref="W156"/>
+      <selection pane="bottomRight" activeCell="AD1" sqref="AD1:AD154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2393,7 +2396,9 @@
       <c r="AC1" s="38" t="s">
         <v>255</v>
       </c>
-      <c r="AD1" s="38"/>
+      <c r="AD1" s="38" t="s">
+        <v>256</v>
+      </c>
       <c r="AE1" s="38"/>
       <c r="DH1" s="6"/>
       <c r="XEO1" s="39"/>
@@ -17253,7 +17258,7 @@
       </c>
       <c r="E88" s="52">
         <f t="shared" ca="1" si="8"/>
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F88" s="17">
         <v>100</v>
@@ -17330,7 +17335,9 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="AD88" s="17"/>
+      <c r="AD88" s="17">
+        <v>2</v>
+      </c>
       <c r="AE88" s="17"/>
       <c r="AF88" s="56"/>
       <c r="AG88" s="56"/>
@@ -17443,7 +17450,7 @@
       </c>
       <c r="E89" s="52">
         <f t="shared" ca="1" si="8"/>
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F89" s="17">
         <v>50</v>
@@ -17520,7 +17527,9 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="AD89" s="17"/>
+      <c r="AD89" s="17">
+        <v>1</v>
+      </c>
       <c r="AE89" s="17"/>
       <c r="AF89" s="56"/>
       <c r="AG89" s="56"/>
@@ -24619,7 +24628,9 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AD128" s="45"/>
+      <c r="AD128" s="45">
+        <v>6</v>
+      </c>
       <c r="AE128" s="45"/>
       <c r="XEO128" s="42"/>
       <c r="XEP128" s="42"/>
@@ -24729,7 +24740,9 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AD129" s="45"/>
+      <c r="AD129" s="45">
+        <v>2</v>
+      </c>
       <c r="AE129" s="45"/>
       <c r="XEO129" s="42"/>
       <c r="XEP129" s="42"/>
@@ -24839,7 +24852,9 @@
         <f t="shared" ref="AC130:AC154" si="21">IF(AB130=$S130,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AD130" s="45"/>
+      <c r="AD130" s="45">
+        <v>4</v>
+      </c>
       <c r="AE130" s="45"/>
       <c r="AF130" s="29"/>
       <c r="AG130" s="29"/>
@@ -25029,7 +25044,9 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AD131" s="45"/>
+      <c r="AD131" s="45">
+        <v>5</v>
+      </c>
       <c r="AE131" s="45"/>
       <c r="AF131" s="37"/>
       <c r="AG131" s="37"/>
@@ -25219,7 +25236,9 @@
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="AD132" s="45"/>
+      <c r="AD132" s="45">
+        <v>3</v>
+      </c>
       <c r="AE132" s="45"/>
       <c r="AF132" s="29"/>
       <c r="AG132" s="29"/>
@@ -25409,7 +25428,9 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AD133" s="45"/>
+      <c r="AD133" s="45">
+        <v>1</v>
+      </c>
       <c r="AE133" s="45"/>
       <c r="AF133" s="29"/>
       <c r="AG133" s="29"/>
@@ -44550,7 +44571,7 @@
       </c>
       <c r="E61" s="52">
         <f t="shared" ca="1" si="7"/>
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F61" s="17">
         <v>50</v>
@@ -44627,7 +44648,7 @@
       </c>
       <c r="E62" s="52">
         <f t="shared" ca="1" si="7"/>
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F62" s="17">
         <v>100</v>

</xml_diff>

<commit_message>
ready to test od again
</commit_message>
<xml_diff>
--- a/Database of all images.xlsx
+++ b/Database of all images.xlsx
@@ -1899,11 +1899,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="225441728"/>
-        <c:axId val="225442120"/>
+        <c:axId val="295009792"/>
+        <c:axId val="295010576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="225441728"/>
+        <c:axId val="295009792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1912,7 +1912,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="225442120"/>
+        <c:crossAx val="295010576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1920,7 +1920,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="225442120"/>
+        <c:axId val="295010576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1931,7 +1931,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="225441728"/>
+        <c:crossAx val="295009792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2273,10 +2273,10 @@
   <dimension ref="A1:XFC172"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="T137" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AD1" sqref="AD1:AD154"/>
+      <selection pane="bottomRight" activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7106,7 +7106,7 @@
       </c>
       <c r="E27" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F27" s="45">
         <v>20</v>
@@ -7296,7 +7296,7 @@
       </c>
       <c r="E28" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F28" s="45">
         <v>20</v>
@@ -7406,7 +7406,7 @@
       </c>
       <c r="E29" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F29" s="45">
         <v>20</v>
@@ -7596,7 +7596,7 @@
       </c>
       <c r="E30" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F30" s="45">
         <v>40</v>
@@ -7786,7 +7786,7 @@
       </c>
       <c r="E31" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F31" s="45">
         <v>40</v>
@@ -7976,7 +7976,7 @@
       </c>
       <c r="E32" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F32" s="45">
         <v>30</v>
@@ -38050,7 +38050,7 @@
       </c>
       <c r="E21" s="44">
         <f t="shared" ca="1" si="2"/>
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F21" s="45">
         <v>20</v>
@@ -38220,7 +38220,7 @@
       </c>
       <c r="E22" s="44">
         <f t="shared" ca="1" si="2"/>
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F22" s="45">
         <v>20</v>

</xml_diff>